<commit_message>
BAP tedarikleri ile ilgili çalışmalar.
</commit_message>
<xml_diff>
--- a/Project/BAP/Procurement/bütçe-update.xlsx
+++ b/Project/BAP/Procurement/bütçe-update.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="73">
   <si>
     <t>No</t>
   </si>
@@ -136,14 +136,122 @@
     <t>Rezistif yük</t>
   </si>
   <si>
-    <t>Yıldırım'a mail atıldı</t>
+    <t>Endüktif yük</t>
+  </si>
+  <si>
+    <t>Tedarik adı</t>
+  </si>
+  <si>
+    <t>Miktar</t>
+  </si>
+  <si>
+    <t>Birim</t>
+  </si>
+  <si>
+    <t>Fiyat</t>
+  </si>
+  <si>
+    <t>KDV dahil</t>
+  </si>
+  <si>
+    <t>Firma</t>
+  </si>
+  <si>
+    <t>Yıldırım</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Teklif</t>
+  </si>
+  <si>
+    <t>Earsis</t>
+  </si>
+  <si>
+    <t>Baskı devre kartı dizgisi</t>
+  </si>
+  <si>
+    <t>TŞ</t>
+  </si>
+  <si>
+    <t>Hazırla</t>
+  </si>
+  <si>
+    <t>Sözleşme</t>
+  </si>
+  <si>
+    <t>Doğrultucu soğutucu</t>
+  </si>
+  <si>
+    <t>Analiz</t>
+  </si>
+  <si>
+    <t>http://tr.farnell.com/vishay/vs-26mt100/bridge-rectifier-25a-3ph/dp/9098550</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Kodu</t>
+  </si>
+  <si>
+    <t>AMC1100</t>
+  </si>
+  <si>
+    <t>AMC1200</t>
+  </si>
+  <si>
+    <t>VS-26MT100</t>
+  </si>
+  <si>
+    <t>http://tr.farnell.com/texas-instruments/amc1100dub/amp-isolation-60khz-4-25kviso/dp/2144250</t>
+  </si>
+  <si>
+    <t>http://tr.farnell.com/texas-instruments/amc1200bdwv/ic-isolation-amp-60khz-soic-8/dp/2373533</t>
+  </si>
+  <si>
+    <t>B32778G4107</t>
+  </si>
+  <si>
+    <t>GS66508B</t>
+  </si>
+  <si>
+    <t>https://www.gansystems.com/transistors.php</t>
+  </si>
+  <si>
+    <t>Evirici soğutucu</t>
+  </si>
+  <si>
+    <t>Tasarım</t>
+  </si>
+  <si>
+    <t>Doğrultucu, DC bara giriş</t>
+  </si>
+  <si>
+    <t>Sürücü güç katı</t>
+  </si>
+  <si>
+    <t>Ölçümler</t>
+  </si>
+  <si>
+    <t>Kontrol</t>
+  </si>
+  <si>
+    <t>Kapı sürücü</t>
+  </si>
+  <si>
+    <t>Motor</t>
+  </si>
+  <si>
+    <t>Güç kaynağı</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,16 +282,73 @@
       <family val="2"/>
       <charset val="162"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -243,11 +408,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -288,8 +480,122 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -568,27 +874,1119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="89.5703125" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:11" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="23">
+        <v>1</v>
+      </c>
+      <c r="F2" s="36">
+        <v>2825</v>
+      </c>
+      <c r="G2" s="36">
+        <f>E2*F2</f>
+        <v>2825</v>
+      </c>
+      <c r="H2" s="36">
+        <f>1.18*G2</f>
+        <v>3333.5</v>
+      </c>
+      <c r="I2" s="36"/>
+      <c r="J2" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>36</v>
       </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="23">
+        <v>1</v>
+      </c>
+      <c r="F3" s="36">
+        <v>2875</v>
+      </c>
+      <c r="G3" s="36">
+        <f t="shared" ref="G3" si="0">E3*F3</f>
+        <v>2875</v>
+      </c>
+      <c r="H3" s="36">
+        <f t="shared" ref="H3:H4" si="1">1.18*G3</f>
+        <v>3392.5</v>
+      </c>
+      <c r="I3" s="36"/>
+      <c r="J3" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3" s="38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23">
+        <f t="shared" ref="G4" si="2">E4*F4</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="38"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="36">
+        <f>SUM(H2:H4)</f>
+        <v>6726</v>
+      </c>
+      <c r="I5" s="36">
+        <v>6500</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="38"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="45"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="39"/>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="23">
+        <v>2</v>
+      </c>
+      <c r="F7" s="36">
+        <v>1900</v>
+      </c>
+      <c r="G7" s="36">
+        <f>E7*F7</f>
+        <v>3800</v>
+      </c>
+      <c r="H7" s="36">
+        <f>1.18*G7</f>
+        <v>4484</v>
+      </c>
+      <c r="I7" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="23">
+        <v>2</v>
+      </c>
+      <c r="F8" s="36">
+        <v>850</v>
+      </c>
+      <c r="G8" s="36">
+        <f t="shared" ref="G8:G9" si="3">E8*F8</f>
+        <v>1700</v>
+      </c>
+      <c r="H8" s="36">
+        <f>1.18*G8</f>
+        <v>2006</v>
+      </c>
+      <c r="I8" s="42"/>
+      <c r="J8" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="23">
+        <f>1.18*G9</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="38"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="36">
+        <f>SUM(H7:H9)</f>
+        <v>6490</v>
+      </c>
+      <c r="I10" s="36">
+        <v>6500</v>
+      </c>
+      <c r="J10" s="23"/>
+      <c r="K10" s="38"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="39"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="53"/>
+      <c r="F12" s="53"/>
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="23">
+        <v>2</v>
+      </c>
+      <c r="F13" s="36">
+        <v>57</v>
+      </c>
+      <c r="G13" s="36">
+        <f>E13*F13</f>
+        <v>114</v>
+      </c>
+      <c r="H13" s="36">
+        <f>1.18*G13</f>
+        <v>134.51999999999998</v>
+      </c>
+      <c r="I13" s="36"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="23"/>
+      <c r="D14" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="23">
+        <v>6</v>
+      </c>
+      <c r="F14" s="36">
+        <v>50</v>
+      </c>
+      <c r="G14" s="36">
+        <f>E14*F14</f>
+        <v>300</v>
+      </c>
+      <c r="H14" s="36">
+        <f>1.18*G14</f>
+        <v>354</v>
+      </c>
+      <c r="I14" s="36"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="52" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="23">
+        <v>2</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="36">
+        <f>E15*F15</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="36">
+        <f>1.18*G15</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="J15" s="23"/>
+      <c r="K15" s="50"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="49"/>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="49"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="23">
+        <v>0</v>
+      </c>
+      <c r="F18" s="36">
+        <v>65</v>
+      </c>
+      <c r="G18" s="36">
+        <f>E18*F18</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="36">
+        <f>1.18*G18</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="36"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="23">
+        <v>10</v>
+      </c>
+      <c r="F19" s="36">
+        <v>110</v>
+      </c>
+      <c r="G19" s="36">
+        <f>E19*F19</f>
+        <v>1100</v>
+      </c>
+      <c r="H19" s="36">
+        <f>1.18*G19</f>
+        <v>1298</v>
+      </c>
+      <c r="I19" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="J19" s="23"/>
+      <c r="K19" s="50"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="36">
+        <f>E20*F20</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="36">
+        <f>1.18*G20</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="36"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="50"/>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="51"/>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="53"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="51"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="23"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36">
+        <f>E23*F23</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="36">
+        <f>1.18*G23</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="36"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="50"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" s="23">
+        <v>20</v>
+      </c>
+      <c r="F24" s="36">
+        <v>22.5</v>
+      </c>
+      <c r="G24" s="36">
+        <f>E24*F24</f>
+        <v>450</v>
+      </c>
+      <c r="H24" s="36">
+        <f>1.18*G24</f>
+        <v>531</v>
+      </c>
+      <c r="I24" s="36"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="49" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="51"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="51"/>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="51"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="23"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36">
+        <f>E30*F30</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="36">
+        <f>1.18*G30</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="36"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="50"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="23">
+        <v>5</v>
+      </c>
+      <c r="F31" s="36">
+        <v>22.5</v>
+      </c>
+      <c r="G31" s="36">
+        <f>E31*F31</f>
+        <v>112.5</v>
+      </c>
+      <c r="H31" s="36">
+        <f>1.18*G31</f>
+        <v>132.75</v>
+      </c>
+      <c r="I31" s="36"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+    </row>
+    <row r="34" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="24"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="53"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="23"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36">
+        <f>E36*F36</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="36">
+        <f>1.18*G36</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="36"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="50"/>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="24"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+      <c r="J38" s="24"/>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="24"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="55"/>
+      <c r="C41" s="55"/>
+      <c r="D41" s="55"/>
+      <c r="E41" s="55"/>
+      <c r="F41" s="55"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="55"/>
+      <c r="I41" s="55"/>
+      <c r="J41" s="56"/>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="24"/>
+      <c r="F42" s="24"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="24"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="24"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="36">
+        <f t="shared" ref="G46:G52" si="4">E46*F46</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="36">
+        <f t="shared" ref="H46:H52" si="5">1.18*G46</f>
+        <v>0</v>
+      </c>
+      <c r="I46" s="36"/>
+      <c r="J46" s="23"/>
+      <c r="K46" s="50"/>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="34"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="34"/>
+      <c r="G47" s="34"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="35"/>
+      <c r="K47" s="50"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" s="23"/>
+      <c r="F48" s="23"/>
+      <c r="G48" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H48" s="36">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="36"/>
+      <c r="J48" s="23"/>
+      <c r="K48" s="50"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H49" s="36">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I49" s="36"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="50"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H50" s="36">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I50" s="36"/>
+      <c r="J50" s="23"/>
+      <c r="K50" s="50"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="23"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51" s="23"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H51" s="36">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I51" s="36"/>
+      <c r="J51" s="23"/>
+      <c r="K51" s="50"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" s="23"/>
+      <c r="C52" s="23"/>
+      <c r="D52" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E52" s="23"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H52" s="36">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I52" s="36"/>
+      <c r="J52" s="23"/>
+      <c r="K52" s="50"/>
+    </row>
+    <row r="53" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="27"/>
+      <c r="G53" s="28"/>
+      <c r="H53" s="36">
+        <f>SUM(H12:H27)</f>
+        <v>2317.52</v>
+      </c>
+      <c r="I53" s="36">
+        <v>5500</v>
+      </c>
+      <c r="J53" s="23"/>
+      <c r="K53" s="38"/>
     </row>
   </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A22:J22"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A35:J35"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A53:G53"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A47:J47"/>
+    <mergeCell ref="A41:J41"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K31" r:id="rId1"/>
+    <hyperlink ref="K24" r:id="rId2"/>
+    <hyperlink ref="K18" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -599,8 +1997,8 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1291,7 +2689,7 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
dc link and rectifier design. selection of components for BAP project.
</commit_message>
<xml_diff>
--- a/Project/BAP/Procurement/bütçe-update.xlsx
+++ b/Project/BAP/Procurement/bütçe-update.xlsx
@@ -15,6 +15,7 @@
     <sheet name="alımlar" sheetId="2" r:id="rId1"/>
     <sheet name="plan (2)" sheetId="3" r:id="rId2"/>
     <sheet name="plan" sheetId="1" r:id="rId3"/>
+    <sheet name="others" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="81">
   <si>
     <t>No</t>
   </si>
@@ -184,9 +185,6 @@
     <t>Doğrultucu soğutucu</t>
   </si>
   <si>
-    <t>Analiz</t>
-  </si>
-  <si>
     <t>http://tr.farnell.com/vishay/vs-26mt100/bridge-rectifier-25a-3ph/dp/9098550</t>
   </si>
   <si>
@@ -245,6 +243,33 @@
   </si>
   <si>
     <t>Güç kaynağı</t>
+  </si>
+  <si>
+    <t>Alka</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>http://tr.farnell.com/fischer-elektronik/sk-100-100-sa/heat-sink-100mm-1-5-c-w/dp/4621839</t>
+  </si>
+  <si>
+    <t>http://tr.farnell.com/fischer-elektronik/sk-85-75-sa/heat-sink-75mm-1-2-c-w/dp/4621852</t>
+  </si>
+  <si>
+    <t>Heat sink</t>
+  </si>
+  <si>
+    <t>SK 100/100 SA</t>
+  </si>
+  <si>
+    <t>Fan</t>
+  </si>
+  <si>
+    <t>http://tr.farnell.com/multicomp/mc36260/fan-50x50x10mm-5vdc/dp/1924858</t>
+  </si>
+  <si>
+    <t>http://tr.farnell.com/multicomp/mc36257/fan-40x40x10mm-12vdc/dp/1924856</t>
   </si>
 </sst>
 </file>
@@ -316,7 +341,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -344,6 +369,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -439,7 +470,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -462,24 +493,6 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -500,6 +513,72 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -509,18 +588,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -530,60 +597,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -593,6 +606,31 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -877,1116 +915,1124 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="89.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="89.5703125" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:11" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="K1" s="15" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="17">
         <v>1</v>
       </c>
-      <c r="F2" s="36">
+      <c r="F2" s="23">
         <v>2825</v>
       </c>
-      <c r="G2" s="36">
+      <c r="G2" s="23">
         <f>E2*F2</f>
         <v>2825</v>
       </c>
-      <c r="H2" s="36">
+      <c r="H2" s="23">
         <f>1.18*G2</f>
         <v>3333.5</v>
       </c>
-      <c r="I2" s="36"/>
-      <c r="J2" s="40" t="s">
+      <c r="I2" s="23"/>
+      <c r="J2" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23" t="s">
+      <c r="C3" s="16"/>
+      <c r="D3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="17">
         <v>1</v>
       </c>
-      <c r="F3" s="36">
+      <c r="F3" s="23">
         <v>2875</v>
       </c>
-      <c r="G3" s="36">
+      <c r="G3" s="23">
         <f t="shared" ref="G3" si="0">E3*F3</f>
         <v>2875</v>
       </c>
-      <c r="H3" s="36">
+      <c r="H3" s="23">
         <f t="shared" ref="H3:H4" si="1">1.18*G3</f>
         <v>3392.5</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="40" t="s">
+      <c r="I3" s="23"/>
+      <c r="J3" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23">
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17">
         <f t="shared" ref="G4" si="2">E4*F4</f>
         <v>0</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="38"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="25"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="36">
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="23">
         <f>SUM(H2:H4)</f>
         <v>6726</v>
       </c>
-      <c r="I5" s="36">
+      <c r="I5" s="23">
         <v>6500</v>
       </c>
-      <c r="J5" s="23"/>
-      <c r="K5" s="38"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="25"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="39"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="26"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="17">
         <v>2</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="23">
         <v>1900</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="23">
         <f>E7*F7</f>
         <v>3800</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="23">
         <f>1.18*G7</f>
         <v>4484</v>
       </c>
-      <c r="I7" s="41" t="s">
+      <c r="I7" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="J7" s="40" t="s">
+      <c r="J7" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="K7" s="38" t="s">
+      <c r="K7" s="25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23" t="s">
+      <c r="C8" s="16"/>
+      <c r="D8" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="17">
         <v>2</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="23">
         <v>850</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8" s="23">
         <f t="shared" ref="G8:G9" si="3">E8*F8</f>
         <v>1700</v>
       </c>
-      <c r="H8" s="36">
+      <c r="H8" s="23">
         <f>1.18*G8</f>
         <v>2006</v>
       </c>
-      <c r="I8" s="42"/>
-      <c r="J8" s="40" t="s">
+      <c r="I8" s="39"/>
+      <c r="J8" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="K8" s="38" t="s">
+      <c r="K8" s="25" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="17">
         <f>1.18*G9</f>
         <v>0</v>
       </c>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="38"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="25"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="36">
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="23">
         <f>SUM(H7:H9)</f>
         <v>6490</v>
       </c>
-      <c r="I10" s="36">
+      <c r="I10" s="23">
         <v>6500</v>
       </c>
-      <c r="J10" s="23"/>
-      <c r="K10" s="38"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="25"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="39"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="26"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
+      <c r="A12" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="23" t="s">
+      <c r="A13" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="23" t="s">
+      <c r="C13" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="17">
         <v>2</v>
       </c>
-      <c r="F13" s="36">
+      <c r="F13" s="23">
         <v>57</v>
       </c>
-      <c r="G13" s="36">
+      <c r="G13" s="23">
         <f>E13*F13</f>
         <v>114</v>
       </c>
-      <c r="H13" s="36">
+      <c r="H13" s="23">
         <f>1.18*G13</f>
         <v>134.51999999999998</v>
       </c>
-      <c r="I13" s="36"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="49" t="s">
-        <v>53</v>
+      <c r="I13" s="23"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="34" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" s="23" t="s">
+      <c r="A14" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="23">
+      <c r="C14" s="17"/>
+      <c r="D14" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" s="17">
         <v>6</v>
       </c>
-      <c r="F14" s="36">
+      <c r="F14" s="23">
         <v>50</v>
       </c>
-      <c r="G14" s="36">
+      <c r="G14" s="23">
         <f>E14*F14</f>
         <v>300</v>
       </c>
-      <c r="H14" s="36">
+      <c r="H14" s="23">
         <f>1.18*G14</f>
         <v>354</v>
       </c>
-      <c r="I14" s="36"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="52" t="s">
-        <v>54</v>
+      <c r="I14" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="J14" s="17"/>
+      <c r="K14" s="37" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="23" t="s">
+      <c r="A15" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23" t="s">
+      <c r="C15" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="17">
         <v>2</v>
       </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="36">
+      <c r="F15" s="17">
+        <v>50</v>
+      </c>
+      <c r="G15" s="23">
         <f>E15*F15</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="36">
+        <v>100</v>
+      </c>
+      <c r="H15" s="23">
         <f>1.18*G15</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="J15" s="23"/>
-      <c r="K15" s="50"/>
+        <v>118</v>
+      </c>
+      <c r="I15" s="58"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="34" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="49"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="34"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="49"/>
+      <c r="A17" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="34"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="23" t="s">
+      <c r="A18" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="17">
+        <v>0</v>
+      </c>
+      <c r="F18" s="23">
+        <v>65</v>
+      </c>
+      <c r="G18" s="23">
+        <f>E18*F18</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="23">
+        <f>1.18*G18</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="23"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="23">
-        <v>0</v>
-      </c>
-      <c r="F18" s="36">
-        <v>65</v>
-      </c>
-      <c r="G18" s="36">
-        <f>E18*F18</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="36">
-        <f>1.18*G18</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="36"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="49" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="23" t="s">
+      <c r="A19" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="23" t="s">
+      <c r="C19" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="17">
         <v>10</v>
       </c>
-      <c r="F19" s="36">
+      <c r="F19" s="23">
         <v>110</v>
       </c>
-      <c r="G19" s="36">
+      <c r="G19" s="23">
         <f>E19*F19</f>
         <v>1100</v>
       </c>
-      <c r="H19" s="36">
+      <c r="H19" s="23">
         <f>1.18*G19</f>
         <v>1298</v>
       </c>
-      <c r="I19" s="44" t="s">
-        <v>65</v>
-      </c>
-      <c r="J19" s="23"/>
-      <c r="K19" s="50"/>
+      <c r="I19" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" s="17"/>
+      <c r="K19" s="35"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="23" t="s">
+      <c r="A20" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="36">
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="23">
         <f>E20*F20</f>
         <v>0</v>
       </c>
-      <c r="H20" s="36">
+      <c r="H20" s="23">
         <f>1.18*G20</f>
         <v>0</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="50"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="35"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="51"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="36"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="53" t="s">
-        <v>68</v>
-      </c>
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="51"/>
+      <c r="A22" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="36"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="23" t="s">
+      <c r="A23" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23" t="s">
+      <c r="C23" s="17"/>
+      <c r="D23" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="23"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36">
+      <c r="E23" s="17"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23">
         <f>E23*F23</f>
         <v>0</v>
       </c>
-      <c r="H23" s="36">
+      <c r="H23" s="23">
         <f>1.18*G23</f>
         <v>0</v>
       </c>
-      <c r="I23" s="36"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="50"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="35"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="23" t="s">
+      <c r="A24" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="23" t="s">
+      <c r="C24" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="17">
         <v>20</v>
       </c>
-      <c r="F24" s="36">
+      <c r="F24" s="23">
         <v>22.5</v>
       </c>
-      <c r="G24" s="36">
+      <c r="G24" s="23">
         <f>E24*F24</f>
         <v>450</v>
       </c>
-      <c r="H24" s="36">
+      <c r="H24" s="23">
         <f>1.18*G24</f>
         <v>531</v>
       </c>
-      <c r="I24" s="36"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="49" t="s">
-        <v>60</v>
+      <c r="I24" s="23"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="34" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="51"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="36"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="24"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="51"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="36"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="51"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="36"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="53" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="53"/>
-      <c r="C29" s="53"/>
-      <c r="D29" s="53"/>
-      <c r="E29" s="53"/>
-      <c r="F29" s="53"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="53"/>
+      <c r="A29" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="23" t="s">
+      <c r="A30" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23" t="s">
+      <c r="C30" s="17"/>
+      <c r="D30" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="23"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36">
+      <c r="E30" s="17"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23">
         <f>E30*F30</f>
         <v>0</v>
       </c>
-      <c r="H30" s="36">
+      <c r="H30" s="23">
         <f>1.18*G30</f>
         <v>0</v>
       </c>
-      <c r="I30" s="36"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="50"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="35"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="23" t="s">
+      <c r="A31" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="23" t="s">
+      <c r="C31" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="23">
+      <c r="E31" s="17">
         <v>5</v>
       </c>
-      <c r="F31" s="36">
+      <c r="F31" s="23">
         <v>22.5</v>
       </c>
-      <c r="G31" s="36">
+      <c r="G31" s="23">
         <f>E31*F31</f>
         <v>112.5</v>
       </c>
-      <c r="H31" s="36">
+      <c r="H31" s="23">
         <f>1.18*G31</f>
         <v>132.75</v>
       </c>
-      <c r="I31" s="36"/>
-      <c r="J31" s="23"/>
-      <c r="K31" s="49" t="s">
-        <v>59</v>
+      <c r="I31" s="23"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="34" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="53" t="s">
+      <c r="A35" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="40"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="17"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23">
+        <f>E36*F36</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="23">
+        <f>1.18*G36</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="23"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="35"/>
+    </row>
+    <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="49"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="50"/>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="18"/>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="23">
+        <f t="shared" ref="G46:G52" si="4">E46*F46</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="23">
+        <f t="shared" ref="H46:H52" si="5">1.18*G46</f>
+        <v>0</v>
+      </c>
+      <c r="I46" s="23"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="35"/>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
-      <c r="G35" s="53"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23" t="s">
+      <c r="B47" s="46"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
+      <c r="J47" s="47"/>
+      <c r="K47" s="35"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" s="17"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36">
-        <f>E36*F36</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="36">
-        <f>1.18*G36</f>
-        <v>0</v>
-      </c>
-      <c r="I36" s="36"/>
-      <c r="J36" s="23"/>
-      <c r="K36" s="50"/>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-    </row>
-    <row r="38" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24"/>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="24"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-    </row>
-    <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="54" t="s">
-        <v>72</v>
-      </c>
-      <c r="B41" s="55"/>
-      <c r="C41" s="55"/>
-      <c r="D41" s="55"/>
-      <c r="E41" s="55"/>
-      <c r="F41" s="55"/>
-      <c r="G41" s="55"/>
-      <c r="H41" s="55"/>
-      <c r="I41" s="55"/>
-      <c r="J41" s="56"/>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
-    </row>
-    <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="24"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24"/>
-    </row>
-    <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="24"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-    </row>
-    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="24"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B46" s="23"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23" t="s">
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H48" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="23"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="35"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="36">
-        <f t="shared" ref="G46:G52" si="4">E46*F46</f>
-        <v>0</v>
-      </c>
-      <c r="H46" s="36">
-        <f t="shared" ref="H46:H52" si="5">1.18*G46</f>
-        <v>0</v>
-      </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="23"/>
-      <c r="K46" s="50"/>
-    </row>
-    <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="34"/>
-      <c r="I47" s="34"/>
-      <c r="J47" s="35"/>
-      <c r="K47" s="50"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23" t="s">
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H49" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I49" s="23"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="35"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="17"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E48" s="23"/>
-      <c r="F48" s="23"/>
-      <c r="G48" s="36">
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="23">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H48" s="36">
+      <c r="H50" s="23">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I48" s="36"/>
-      <c r="J48" s="23"/>
-      <c r="K48" s="50"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23" t="s">
+      <c r="I50" s="23"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="35"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="17"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E49" s="23"/>
-      <c r="F49" s="23"/>
-      <c r="G49" s="36">
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="23">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H49" s="36">
+      <c r="H51" s="23">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I49" s="36"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="50"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23" t="s">
+      <c r="I51" s="23"/>
+      <c r="J51" s="17"/>
+      <c r="K51" s="35"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" s="17"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="36">
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="23">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H50" s="36">
+      <c r="H52" s="23">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="I50" s="36"/>
-      <c r="J50" s="23"/>
-      <c r="K50" s="50"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B51" s="23"/>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E51" s="23"/>
-      <c r="F51" s="23"/>
-      <c r="G51" s="36">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H51" s="36">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I51" s="36"/>
-      <c r="J51" s="23"/>
-      <c r="K51" s="50"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B52" s="23"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="36">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H52" s="36">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I52" s="36"/>
-      <c r="J52" s="23"/>
-      <c r="K52" s="50"/>
+      <c r="I52" s="23"/>
+      <c r="J52" s="17"/>
+      <c r="K52" s="35"/>
     </row>
     <row r="53" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="26" t="s">
+      <c r="A53" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B53" s="27"/>
-      <c r="C53" s="27"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="28"/>
-      <c r="H53" s="36">
+      <c r="B53" s="43"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="43"/>
+      <c r="E53" s="43"/>
+      <c r="F53" s="43"/>
+      <c r="G53" s="44"/>
+      <c r="H53" s="23">
         <f>SUM(H12:H27)</f>
-        <v>2317.52</v>
-      </c>
-      <c r="I53" s="36">
+        <v>2435.52</v>
+      </c>
+      <c r="I53" s="23">
         <v>5500</v>
       </c>
-      <c r="J53" s="23"/>
-      <c r="K53" s="38"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="A22:J22"/>
-    <mergeCell ref="A29:J29"/>
     <mergeCell ref="A35:J35"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A53:G53"/>
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="A47:J47"/>
     <mergeCell ref="A41:J41"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A22:J22"/>
+    <mergeCell ref="A29:J29"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K31" r:id="rId1"/>
     <hyperlink ref="K24" r:id="rId2"/>
     <hyperlink ref="K18" r:id="rId3"/>
+    <hyperlink ref="K13" r:id="rId4"/>
+    <hyperlink ref="K15" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -2138,15 +2184,15 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="53"/>
       <c r="H5" s="8">
         <f>SUM(H2:H4)</f>
         <v>6608</v>
@@ -2528,15 +2574,15 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="17"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="56"/>
       <c r="H19" s="8">
         <f>SUM(H7:H18)</f>
         <v>3091.6</v>
@@ -2657,15 +2703,15 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="17"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="56"/>
       <c r="H25" s="9">
         <f>SUM(H21:H24)</f>
         <v>5900</v>
@@ -2830,15 +2876,15 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="14"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="53"/>
       <c r="H5" s="8">
         <f>SUM(H2:H4)</f>
         <v>6608</v>
@@ -3220,15 +3266,15 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="17"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="56"/>
       <c r="H19" s="8">
         <f>SUM(H7:H18)</f>
         <v>5097.5999999999995</v>
@@ -3349,15 +3395,15 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="17"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="56"/>
       <c r="H25" s="9">
         <f>SUM(H21:H24)</f>
         <v>5900</v>
@@ -3372,4 +3418,59 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="82.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="59" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="59" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="59" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A6" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
BAP alımları ile ilgili çalışmalar. dc link inductor tasarımı, kapasitör seçimi.
</commit_message>
<xml_diff>
--- a/Project/BAP/Procurement/bütçe-update.xlsx
+++ b/Project/BAP/Procurement/bütçe-update.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="85">
   <si>
     <t>No</t>
   </si>
@@ -273,6 +273,15 @@
   </si>
   <si>
     <t>DC kondansatör</t>
+  </si>
+  <si>
+    <t>http://tr.farnell.com/epcos/b43456a4228m000/cap-alu-elec-2200uf-350v-screw/dp/2284036</t>
+  </si>
+  <si>
+    <t>B43630A9128</t>
+  </si>
+  <si>
+    <t>Seç</t>
   </si>
 </sst>
 </file>
@@ -567,6 +576,43 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -574,37 +620,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -624,13 +640,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -912,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,7 +1121,7 @@
         <f>1.18*G7</f>
         <v>4484</v>
       </c>
-      <c r="I7" s="37" t="s">
+      <c r="I7" s="50" t="s">
         <v>50</v>
       </c>
       <c r="J7" s="27" t="s">
@@ -1147,7 +1156,7 @@
         <f>1.18*G8</f>
         <v>2006</v>
       </c>
-      <c r="I8" s="38"/>
+      <c r="I8" s="51"/>
       <c r="J8" s="27" t="s">
         <v>49</v>
       </c>
@@ -1210,18 +1219,18 @@
       <c r="K11" s="26"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
@@ -1264,25 +1273,25 @@
         <v>12</v>
       </c>
       <c r="C14" s="17"/>
-      <c r="D14" s="56" t="s">
-        <v>72</v>
+      <c r="D14" s="17" t="s">
+        <v>43</v>
       </c>
       <c r="E14" s="17">
         <v>6</v>
       </c>
       <c r="F14" s="23">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="G14" s="23">
         <f>E14*F14</f>
-        <v>300</v>
+        <v>516</v>
       </c>
       <c r="H14" s="23">
         <f>1.18*G14</f>
-        <v>354</v>
+        <v>608.88</v>
       </c>
       <c r="I14" s="28" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="J14" s="17"/>
       <c r="K14" s="36" t="s">
@@ -1294,32 +1303,32 @@
         <v>25</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>43</v>
+        <v>12</v>
+      </c>
+      <c r="C15" s="17"/>
+      <c r="D15" s="37" t="s">
+        <v>72</v>
       </c>
       <c r="E15" s="17">
-        <v>2</v>
-      </c>
-      <c r="F15" s="17">
-        <v>27</v>
+        <v>6</v>
+      </c>
+      <c r="F15" s="23">
+        <v>50</v>
       </c>
       <c r="G15" s="23">
         <f>E15*F15</f>
-        <v>54</v>
+        <v>300</v>
       </c>
       <c r="H15" s="23">
         <f>1.18*G15</f>
-        <v>63.72</v>
-      </c>
-      <c r="I15" s="57"/>
+        <v>354</v>
+      </c>
+      <c r="I15" s="28" t="s">
+        <v>73</v>
+      </c>
       <c r="J15" s="17"/>
-      <c r="K15" s="33" t="s">
-        <v>74</v>
+      <c r="K15" s="36" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1327,218 +1336,254 @@
         <v>25</v>
       </c>
       <c r="B16" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="17">
+        <v>2</v>
+      </c>
+      <c r="F16" s="17">
+        <v>27</v>
+      </c>
+      <c r="G16" s="23">
+        <f>E16*F16</f>
+        <v>54</v>
+      </c>
+      <c r="H16" s="23">
+        <f>1.18*G16</f>
+        <v>63.72</v>
+      </c>
+      <c r="I16" s="38"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="33"/>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
+      <c r="C17" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="17">
+        <v>10</v>
+      </c>
+      <c r="F17" s="23">
+        <v>50</v>
+      </c>
+      <c r="G17" s="23">
+        <f>E17*F17</f>
+        <v>500</v>
+      </c>
+      <c r="H17" s="23">
+        <f>1.18*G17</f>
+        <v>590</v>
+      </c>
+      <c r="I17" s="23"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="33" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="33"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="56"/>
-      <c r="E18" s="17">
-        <v>0</v>
-      </c>
-      <c r="F18" s="23">
-        <v>65</v>
-      </c>
-      <c r="G18" s="23">
-        <f>E18*F18</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="23">
-        <f>1.18*G18</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="23"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="33" t="s">
-        <v>62</v>
-      </c>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="33"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>43</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D19" s="37"/>
       <c r="E19" s="17">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F19" s="23">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="G19" s="23">
         <f>E19*F19</f>
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="H19" s="23">
         <f>1.18*G19</f>
-        <v>1298</v>
-      </c>
-      <c r="I19" s="28" t="s">
-        <v>64</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I19" s="23"/>
       <c r="J19" s="17"/>
-      <c r="K19" s="34"/>
+      <c r="K19" s="33" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" s="56"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
+        <v>11</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="17">
+        <v>10</v>
+      </c>
+      <c r="F20" s="23">
+        <v>110</v>
+      </c>
       <c r="G20" s="23">
         <f>E20*F20</f>
-        <v>0</v>
+        <v>1100</v>
       </c>
       <c r="H20" s="23">
         <f>1.18*G20</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="23"/>
+        <v>1298</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>64</v>
+      </c>
       <c r="J20" s="17"/>
       <c r="K20" s="34"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="35"/>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="37"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="23">
+        <f>E21*F21</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="23">
+        <f>1.18*G21</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="23"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="34"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="35"/>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="35"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23">
-        <f>E23*F23</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="23">
-        <f>1.18*G23</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="23"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="34"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="35"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>56</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C24" s="17"/>
       <c r="D24" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="17">
-        <v>20</v>
-      </c>
-      <c r="F24" s="23">
-        <v>22.5</v>
-      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="23"/>
       <c r="G24" s="23">
         <f>E24*F24</f>
-        <v>450</v>
+        <v>0</v>
       </c>
       <c r="H24" s="23">
         <f>1.18*G24</f>
-        <v>531</v>
+        <v>0</v>
       </c>
       <c r="I24" s="23"/>
       <c r="J24" s="17"/>
-      <c r="K24" s="33" t="s">
+      <c r="K24" s="34"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="17">
+        <v>20</v>
+      </c>
+      <c r="F25" s="23">
+        <v>22.5</v>
+      </c>
+      <c r="G25" s="23">
+        <f>E25*F25</f>
+        <v>450</v>
+      </c>
+      <c r="H25" s="23">
+        <f>1.18*G25</f>
+        <v>531</v>
+      </c>
+      <c r="I25" s="23"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="33" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="35"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
@@ -1577,90 +1622,91 @@
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
+      <c r="K28" s="35"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23">
-        <f>E30*F30</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="23">
-        <f>1.18*G30</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="23"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="34"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>55</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C31" s="17"/>
       <c r="D31" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="17">
-        <v>5</v>
-      </c>
-      <c r="F31" s="23">
-        <v>22.5</v>
-      </c>
+      <c r="E31" s="17"/>
+      <c r="F31" s="23"/>
       <c r="G31" s="23">
         <f>E31*F31</f>
-        <v>112.5</v>
+        <v>0</v>
       </c>
       <c r="H31" s="23">
         <f>1.18*G31</f>
-        <v>132.75</v>
+        <v>0</v>
       </c>
       <c r="I31" s="23"/>
       <c r="J31" s="17"/>
-      <c r="K31" s="33" t="s">
+      <c r="K31" s="34"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" s="17">
+        <v>5</v>
+      </c>
+      <c r="F32" s="23">
+        <v>22.5</v>
+      </c>
+      <c r="G32" s="23">
+        <f>E32*F32</f>
+        <v>112.5</v>
+      </c>
+      <c r="H32" s="23">
+        <f>1.18*G32</f>
+        <v>132.75</v>
+      </c>
+      <c r="I32" s="23"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="33" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="18"/>
@@ -1687,55 +1733,55 @@
       <c r="J34" s="18"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+    </row>
+    <row r="36" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="39"/>
-      <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17" t="s">
+      <c r="C37" s="17"/>
+      <c r="D37" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E36" s="17"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23">
-        <f>E36*F36</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="23">
-        <f>1.18*G36</f>
-        <v>0</v>
-      </c>
-      <c r="I36" s="23"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="34"/>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
+      <c r="E37" s="17"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23">
+        <f>E37*F37</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="23">
+        <f>1.18*G37</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="23"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="34"/>
     </row>
     <row r="38" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="18"/>
@@ -1774,30 +1820,30 @@
       <c r="J40" s="18"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="47" t="s">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+    </row>
+    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="49"/>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="18"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="18"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="48"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="49"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="18"/>
@@ -1835,65 +1881,54 @@
       <c r="I45" s="18"/>
       <c r="J45" s="18"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B46" s="17"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17" t="s">
+    <row r="46" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="17"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="23">
-        <f t="shared" ref="G46:G52" si="4">E46*F46</f>
-        <v>0</v>
-      </c>
-      <c r="H46" s="23">
-        <f t="shared" ref="H46:H52" si="5">1.18*G46</f>
-        <v>0</v>
-      </c>
-      <c r="I46" s="23"/>
-      <c r="J46" s="17"/>
-      <c r="K46" s="34"/>
-    </row>
-    <row r="47" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="44" t="s">
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="23">
+        <f t="shared" ref="G47:G53" si="4">E47*F47</f>
+        <v>0</v>
+      </c>
+      <c r="H47" s="23">
+        <f t="shared" ref="H47:H53" si="5">1.18*G47</f>
+        <v>0</v>
+      </c>
+      <c r="I47" s="23"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="34"/>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="45"/>
-      <c r="J47" s="46"/>
-      <c r="K47" s="34"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="23">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H48" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I48" s="23"/>
-      <c r="J48" s="17"/>
+      <c r="B48" s="45"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="46"/>
       <c r="K48" s="34"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -1988,46 +2023,69 @@
       <c r="J52" s="17"/>
       <c r="K52" s="34"/>
     </row>
-    <row r="53" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="41" t="s">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="17"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E53" s="17"/>
+      <c r="F53" s="17"/>
+      <c r="G53" s="23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H53" s="23">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I53" s="23"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="34"/>
+    </row>
+    <row r="54" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="B53" s="42"/>
-      <c r="C53" s="42"/>
-      <c r="D53" s="42"/>
-      <c r="E53" s="42"/>
-      <c r="F53" s="42"/>
-      <c r="G53" s="43"/>
-      <c r="H53" s="23">
-        <f>SUM(H12:H27)</f>
-        <v>2381.2399999999998</v>
-      </c>
-      <c r="I53" s="23">
+      <c r="B54" s="42"/>
+      <c r="C54" s="42"/>
+      <c r="D54" s="42"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="43"/>
+      <c r="H54" s="23">
+        <f>SUM(H12:H28)</f>
+        <v>3580.12</v>
+      </c>
+      <c r="I54" s="23">
         <v>5500</v>
       </c>
-      <c r="J53" s="17"/>
-      <c r="K53" s="25"/>
+      <c r="J54" s="17"/>
+      <c r="K54" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A35:J35"/>
+    <mergeCell ref="A36:J36"/>
     <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A53:G53"/>
+    <mergeCell ref="A54:G54"/>
     <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A47:J47"/>
-    <mergeCell ref="A41:J41"/>
+    <mergeCell ref="A48:J48"/>
+    <mergeCell ref="A42:J42"/>
     <mergeCell ref="I7:I8"/>
     <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="A22:J22"/>
-    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A18:J18"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A30:J30"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K31" r:id="rId1"/>
-    <hyperlink ref="K24" r:id="rId2"/>
-    <hyperlink ref="K18" r:id="rId3"/>
+    <hyperlink ref="K32" r:id="rId1"/>
+    <hyperlink ref="K25" r:id="rId2"/>
+    <hyperlink ref="K19" r:id="rId3"/>
     <hyperlink ref="K13" r:id="rId4"/>
-    <hyperlink ref="K15" r:id="rId5"/>
+    <hyperlink ref="K16" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
@@ -2182,15 +2240,15 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="52"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="8">
         <f>SUM(H2:H4)</f>
         <v>6608</v>
@@ -2572,15 +2630,15 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="55"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="58"/>
       <c r="H19" s="8">
         <f>SUM(H7:H18)</f>
         <v>3091.6</v>
@@ -2701,15 +2759,15 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="53" t="s">
+      <c r="A25" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="55"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="58"/>
       <c r="H25" s="9">
         <f>SUM(H21:H24)</f>
         <v>5900</v>
@@ -2874,15 +2932,15 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="52"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="8">
         <f>SUM(H2:H4)</f>
         <v>6608</v>
@@ -3264,15 +3322,15 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="55"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="58"/>
       <c r="H19" s="8">
         <f>SUM(H7:H18)</f>
         <v>5097.5999999999995</v>
@@ -3393,15 +3451,15 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="53" t="s">
+      <c r="A25" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="55"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="58"/>
       <c r="H25" s="9">
         <f>SUM(H21:H24)</f>
         <v>5900</v>
@@ -3437,12 +3495,12 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="39" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="39" t="s">
         <v>74</v>
       </c>
     </row>
@@ -3452,12 +3510,12 @@
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="58" t="s">
+      <c r="A5" s="39" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="39" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
A few small updates.
</commit_message>
<xml_diff>
--- a/Project/BAP/Procurement/bütçe-update.xlsx
+++ b/Project/BAP/Procurement/bütçe-update.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="95">
   <si>
     <t>No</t>
   </si>
@@ -173,33 +173,15 @@
     <t>Baskı devre kartı dizgisi</t>
   </si>
   <si>
-    <t>TŞ</t>
-  </si>
-  <si>
-    <t>Hazırla</t>
-  </si>
-  <si>
-    <t>Sözleşme</t>
-  </si>
-  <si>
     <t>Doğrultucu soğutucu</t>
   </si>
   <si>
     <t>http://tr.farnell.com/vishay/vs-26mt100/bridge-rectifier-25a-3ph/dp/9098550</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>Kodu</t>
   </si>
   <si>
-    <t>AMC1100</t>
-  </si>
-  <si>
-    <t>AMC1200</t>
-  </si>
-  <si>
     <t>VS-26MT100</t>
   </si>
   <si>
@@ -248,9 +230,6 @@
     <t>Alka</t>
   </si>
   <si>
-    <t>Mail</t>
-  </si>
-  <si>
     <t>http://tr.farnell.com/fischer-elektronik/sk-100-100-sa/heat-sink-100mm-1-5-c-w/dp/4621839</t>
   </si>
   <si>
@@ -282,6 +261,57 @@
   </si>
   <si>
     <t>Seç</t>
+  </si>
+  <si>
+    <t>GaN EVM</t>
+  </si>
+  <si>
+    <t>İzole kaynak 5V</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>MCU buffer</t>
+  </si>
+  <si>
+    <t>Sense direnci</t>
+  </si>
+  <si>
+    <t>Konektör</t>
+  </si>
+  <si>
+    <t>9V üretici</t>
+  </si>
+  <si>
+    <t>6V üretici</t>
+  </si>
+  <si>
+    <t>Gate drive entegre</t>
+  </si>
+  <si>
+    <t>Divider dirençleri</t>
+  </si>
+  <si>
+    <t>Flyback entegre</t>
+  </si>
+  <si>
+    <t>Flyback trafo</t>
+  </si>
+  <si>
+    <t>Transistör</t>
+  </si>
+  <si>
+    <t>Diyot</t>
+  </si>
+  <si>
+    <t>Kapasitör</t>
+  </si>
+  <si>
+    <t>MCU supply</t>
+  </si>
+  <si>
+    <t>MU haberleşme</t>
   </si>
 </sst>
 </file>
@@ -353,7 +383,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,18 +398,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -387,6 +405,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -482,7 +506,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -531,25 +555,16 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -558,9 +573,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -573,19 +585,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -596,22 +611,40 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -619,26 +652,32 @@
     <xf numFmtId="2" fontId="6" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -921,66 +960,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K54"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="56" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="56" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.5703125" style="56" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="56" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="89.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="89.5703125" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>54</v>
+      <c r="C1" s="36" t="s">
+        <v>50</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="36" t="s">
         <v>41</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="60" t="s">
         <v>35</v>
       </c>
       <c r="C2" s="16"/>
@@ -990,30 +1025,27 @@
       <c r="E2" s="17">
         <v>1</v>
       </c>
-      <c r="F2" s="23">
-        <v>2825</v>
-      </c>
-      <c r="G2" s="23">
+      <c r="F2" s="22">
+        <v>2625</v>
+      </c>
+      <c r="G2" s="22">
         <f>E2*F2</f>
-        <v>2825</v>
-      </c>
-      <c r="H2" s="23">
+        <v>2625</v>
+      </c>
+      <c r="H2" s="22">
         <f>1.18*G2</f>
-        <v>3333.5</v>
-      </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" s="25" t="s">
+        <v>3097.5</v>
+      </c>
+      <c r="I2" s="22"/>
+      <c r="J2" s="23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="60" t="s">
         <v>36</v>
       </c>
       <c r="C3" s="16"/>
@@ -1023,85 +1055,89 @@
       <c r="E3" s="17">
         <v>1</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="22">
         <v>2875</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="22">
         <f t="shared" ref="G3" si="0">E3*F3</f>
         <v>2875</v>
       </c>
-      <c r="H3" s="23">
-        <f t="shared" ref="H3:H4" si="1">1.18*G3</f>
+      <c r="H3" s="22">
+        <f t="shared" ref="H3" si="1">1.18*G3</f>
         <v>3392.5</v>
       </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="K3" s="25" t="s">
+      <c r="I3" s="22"/>
+      <c r="J3" s="23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17">
-        <f t="shared" ref="G4" si="2">E4*F4</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="25"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="43"/>
-      <c r="H5" s="23">
-        <f>SUM(H2:H4)</f>
-        <v>6726</v>
-      </c>
-      <c r="I5" s="23">
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="22">
+        <f>SUM(H2:H3)</f>
+        <v>6490</v>
+      </c>
+      <c r="I4" s="22">
         <v>6500</v>
       </c>
-      <c r="J5" s="17"/>
-      <c r="K5" s="25"/>
-    </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="26"/>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J4" s="23"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="24"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="17">
+        <v>2</v>
+      </c>
+      <c r="F6" s="22">
+        <v>1900</v>
+      </c>
+      <c r="G6" s="22">
+        <f>E6*F6</f>
+        <v>3800</v>
+      </c>
+      <c r="H6" s="22">
+        <f>1.18*G6</f>
+        <v>4484</v>
+      </c>
+      <c r="I6" s="53"/>
+      <c r="J6" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>20</v>
+      <c r="B7" s="60" t="s">
+        <v>47</v>
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="17" t="s">
@@ -1110,985 +1146,1218 @@
       <c r="E7" s="17">
         <v>2</v>
       </c>
-      <c r="F7" s="23">
-        <v>1900</v>
-      </c>
-      <c r="G7" s="23">
-        <f>E7*F7</f>
-        <v>3800</v>
-      </c>
-      <c r="H7" s="23">
+      <c r="F7" s="22">
+        <v>850</v>
+      </c>
+      <c r="G7" s="22">
+        <f t="shared" ref="G7" si="2">E7*F7</f>
+        <v>1700</v>
+      </c>
+      <c r="H7" s="22">
         <f>1.18*G7</f>
-        <v>4484</v>
-      </c>
-      <c r="I7" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="J7" s="27" t="s">
+        <v>2006</v>
+      </c>
+      <c r="I7" s="54"/>
+      <c r="J7" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="22">
+        <f>SUM(H6:H7)</f>
+        <v>6490</v>
+      </c>
+      <c r="I8" s="22">
+        <v>6500</v>
+      </c>
+      <c r="J8" s="23"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="24"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="37"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="17">
+        <v>2</v>
+      </c>
+      <c r="F11" s="22">
+        <v>57</v>
+      </c>
+      <c r="G11" s="22">
+        <f>E11*F11</f>
+        <v>114</v>
+      </c>
+      <c r="H11" s="22">
+        <f>1.18*G11</f>
+        <v>134.51999999999998</v>
+      </c>
+      <c r="I11" s="22"/>
+      <c r="J11" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="K7" s="25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="17">
-        <v>2</v>
-      </c>
-      <c r="F8" s="23">
-        <v>850</v>
-      </c>
-      <c r="G8" s="23">
-        <f t="shared" ref="G8:G9" si="3">E8*F8</f>
-        <v>1700</v>
-      </c>
-      <c r="H8" s="23">
-        <f>1.18*G8</f>
-        <v>2006</v>
-      </c>
-      <c r="I8" s="51"/>
-      <c r="J8" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="17">
-        <f>1.18*G9</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="25"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="23">
-        <f>SUM(H7:H9)</f>
-        <v>6490</v>
-      </c>
-      <c r="I10" s="23">
-        <v>6500</v>
-      </c>
-      <c r="J10" s="17"/>
-      <c r="K10" s="25"/>
-    </row>
-    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="26"/>
-    </row>
-    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
-        <v>65</v>
-      </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="17" t="s">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="17">
-        <v>2</v>
-      </c>
-      <c r="F13" s="23">
-        <v>57</v>
-      </c>
-      <c r="G13" s="23">
+      <c r="E12" s="17">
+        <v>6</v>
+      </c>
+      <c r="F12" s="22">
+        <v>86</v>
+      </c>
+      <c r="G12" s="22">
+        <f>E12*F12</f>
+        <v>516</v>
+      </c>
+      <c r="H12" s="22">
+        <f>1.18*G12</f>
+        <v>608.88</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="J12" s="32"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="50">
+        <v>0</v>
+      </c>
+      <c r="F13" s="51">
+        <v>0</v>
+      </c>
+      <c r="G13" s="51">
         <f>E13*F13</f>
-        <v>114</v>
-      </c>
-      <c r="H13" s="23">
+        <v>0</v>
+      </c>
+      <c r="H13" s="51">
         <f>1.18*G13</f>
-        <v>134.51999999999998</v>
-      </c>
-      <c r="I13" s="23"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="I13" s="51"/>
+      <c r="J13" s="52"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="17"/>
+      <c r="B14" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>70</v>
+      </c>
       <c r="D14" s="17" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="17">
-        <v>6</v>
-      </c>
-      <c r="F14" s="23">
-        <v>86</v>
-      </c>
-      <c r="G14" s="23">
+        <v>2</v>
+      </c>
+      <c r="F14" s="17">
+        <v>27</v>
+      </c>
+      <c r="G14" s="22">
         <f>E14*F14</f>
-        <v>516</v>
-      </c>
-      <c r="H14" s="23">
+        <v>54</v>
+      </c>
+      <c r="H14" s="22">
         <f>1.18*G14</f>
-        <v>608.88</v>
-      </c>
-      <c r="I14" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="J14" s="17"/>
-      <c r="K14" s="36" t="s">
+        <v>63.72</v>
+      </c>
+      <c r="I14" s="34"/>
+      <c r="J14" s="29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="17">
+        <v>10</v>
+      </c>
+      <c r="F15" s="22">
+        <v>50</v>
+      </c>
+      <c r="G15" s="22">
+        <f>E15*F15</f>
+        <v>500</v>
+      </c>
+      <c r="H15" s="22">
+        <f>1.18*G15</f>
+        <v>590</v>
+      </c>
+      <c r="I15" s="22"/>
+      <c r="J15" s="29" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="29"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="33"/>
+      <c r="E17" s="17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="22">
+        <v>65</v>
+      </c>
+      <c r="G17" s="22">
+        <f>E17*F17</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="22">
+        <f>1.18*G17</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="22"/>
+      <c r="J17" s="29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="17">
+        <v>10</v>
+      </c>
+      <c r="F18" s="22">
+        <v>110</v>
+      </c>
+      <c r="G18" s="22">
+        <f>E18*F18</f>
+        <v>1100</v>
+      </c>
+      <c r="H18" s="22">
+        <f>1.18*G18</f>
+        <v>1298</v>
+      </c>
+      <c r="I18" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" s="30"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="17">
+        <v>0</v>
+      </c>
+      <c r="F19" s="17">
+        <v>0</v>
+      </c>
+      <c r="G19" s="22">
+        <f>E19*F19</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="22">
+        <f>1.18*G19</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="J19" s="30"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="16"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="31"/>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="31"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="17">
+        <v>0</v>
+      </c>
+      <c r="F22" s="22">
+        <v>0</v>
+      </c>
+      <c r="G22" s="22">
+        <f>E22*F22</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="22">
+        <f>1.18*G22</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="22"/>
+      <c r="J22" s="30"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="17">
+        <v>20</v>
+      </c>
+      <c r="F23" s="22">
+        <v>22.5</v>
+      </c>
+      <c r="G23" s="22">
+        <f>E23*F23</f>
+        <v>450</v>
+      </c>
+      <c r="H23" s="22">
+        <f>1.18*G23</f>
+        <v>531</v>
+      </c>
+      <c r="I23" s="22"/>
+      <c r="J23" s="29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="17">
-        <v>6</v>
-      </c>
-      <c r="F15" s="23">
-        <v>50</v>
-      </c>
-      <c r="G15" s="23">
-        <f>E15*F15</f>
-        <v>300</v>
-      </c>
-      <c r="H15" s="23">
-        <f>1.18*G15</f>
-        <v>354</v>
-      </c>
-      <c r="I15" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="J15" s="17"/>
-      <c r="K15" s="36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="17">
-        <v>2</v>
-      </c>
-      <c r="F16" s="17">
-        <v>27</v>
-      </c>
-      <c r="G16" s="23">
-        <f>E16*F16</f>
-        <v>54</v>
-      </c>
-      <c r="H16" s="23">
-        <f>1.18*G16</f>
-        <v>63.72</v>
-      </c>
-      <c r="I16" s="38"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="33" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="17">
-        <v>10</v>
-      </c>
-      <c r="F17" s="23">
-        <v>50</v>
-      </c>
-      <c r="G17" s="23">
-        <f>E17*F17</f>
-        <v>500</v>
-      </c>
-      <c r="H17" s="23">
-        <f>1.18*G17</f>
-        <v>590</v>
-      </c>
-      <c r="I17" s="23"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="33" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="52" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="33"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="17">
-        <v>0</v>
-      </c>
-      <c r="F19" s="23">
-        <v>65</v>
-      </c>
-      <c r="G19" s="23">
-        <f>E19*F19</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="23">
-        <f>1.18*G19</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="23"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="33" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="17">
-        <v>10</v>
-      </c>
-      <c r="F20" s="23">
-        <v>110</v>
-      </c>
-      <c r="G20" s="23">
-        <f>E20*F20</f>
-        <v>1100</v>
-      </c>
-      <c r="H20" s="23">
-        <f>1.18*G20</f>
-        <v>1298</v>
-      </c>
-      <c r="I20" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="J20" s="17"/>
-      <c r="K20" s="34"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="23">
-        <f>E21*F21</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="23">
-        <f>1.18*G21</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="23"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="34"/>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="35"/>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="40" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="35"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="17"/>
+      <c r="B24" s="60" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>80</v>
+      </c>
       <c r="D24" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23">
-        <f>E24*F24</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="23">
-        <f>1.18*G24</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="23"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="34"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E24" s="16">
+        <v>0</v>
+      </c>
+      <c r="F24" s="16">
+        <v>0</v>
+      </c>
+      <c r="G24" s="22">
+        <f t="shared" ref="G24:G27" si="3">E24*F24</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="22">
+        <f t="shared" ref="H24:H27" si="4">1.18*G24</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="18"/>
+      <c r="J24" s="31"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="17" t="s">
-        <v>16</v>
+      <c r="B25" s="23" t="s">
+        <v>15</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>43</v>
       </c>
       <c r="E25" s="17">
-        <v>20</v>
-      </c>
-      <c r="F25" s="23">
+        <v>5</v>
+      </c>
+      <c r="F25" s="22">
         <v>22.5</v>
       </c>
-      <c r="G25" s="23">
-        <f>E25*F25</f>
-        <v>450</v>
-      </c>
-      <c r="H25" s="23">
-        <f>1.18*G25</f>
-        <v>531</v>
-      </c>
-      <c r="I25" s="23"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="33" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
+      <c r="G25" s="22">
+        <f t="shared" si="3"/>
+        <v>112.5</v>
+      </c>
+      <c r="H25" s="22">
+        <f t="shared" si="4"/>
+        <v>132.75</v>
+      </c>
+      <c r="I25" s="18"/>
+      <c r="J25" s="31"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="60" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="16">
+        <v>0</v>
+      </c>
+      <c r="F26" s="16">
+        <v>0</v>
+      </c>
+      <c r="G26" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="35"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
+      <c r="J26" s="31"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="16">
+        <v>0</v>
+      </c>
+      <c r="F27" s="16">
+        <v>0</v>
+      </c>
+      <c r="G27" s="16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="35"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="60"/>
+      <c r="C28" s="16"/>
       <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
       <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="35"/>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-    </row>
-    <row r="30" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" s="17">
+        <v>0</v>
+      </c>
+      <c r="F30" s="22">
+        <v>0</v>
+      </c>
+      <c r="G30" s="22">
+        <f>E30*F30</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="22">
+        <f>1.18*G30</f>
+        <v>0</v>
+      </c>
+      <c r="I30" s="22"/>
+      <c r="J30" s="30"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="17" t="s">
-        <v>17</v>
+      <c r="B31" s="23" t="s">
+        <v>81</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="17"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23">
-        <f>E31*F31</f>
-        <v>0</v>
-      </c>
-      <c r="H31" s="23">
-        <f>1.18*G31</f>
-        <v>0</v>
-      </c>
-      <c r="I31" s="23"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="34"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E31" s="17">
+        <v>0</v>
+      </c>
+      <c r="F31" s="22">
+        <v>0</v>
+      </c>
+      <c r="G31" s="22">
+        <f t="shared" ref="G31:G34" si="5">E31*F31</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="22">
+        <f t="shared" ref="H31:H34" si="6">1.18*G31</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="22"/>
+      <c r="J31" s="29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>55</v>
-      </c>
+      <c r="B32" s="60" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="16"/>
       <c r="D32" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E32" s="17">
-        <v>5</v>
-      </c>
-      <c r="F32" s="23">
-        <v>22.5</v>
-      </c>
-      <c r="G32" s="23">
-        <f>E32*F32</f>
-        <v>112.5</v>
-      </c>
-      <c r="H32" s="23">
-        <f>1.18*G32</f>
-        <v>132.75</v>
-      </c>
-      <c r="I32" s="23"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="33" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
+      <c r="E32" s="16">
+        <v>0</v>
+      </c>
+      <c r="F32" s="16">
+        <v>0</v>
+      </c>
+      <c r="G32" s="22">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="18"/>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="16"/>
+      <c r="D33" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="16">
+        <v>0</v>
+      </c>
+      <c r="F33" s="16">
+        <v>0</v>
+      </c>
+      <c r="G33" s="22">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H33" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-    </row>
-    <row r="34" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
+    </row>
+    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="60"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="16">
+        <v>0</v>
+      </c>
+      <c r="F34" s="16">
+        <v>0</v>
+      </c>
+      <c r="G34" s="22">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
       <c r="I34" s="18"/>
-      <c r="J34" s="18"/>
-    </row>
-    <row r="35" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-    </row>
-    <row r="36" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="40"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="17">
+        <v>0</v>
+      </c>
+      <c r="F36" s="22">
+        <v>0</v>
+      </c>
+      <c r="G36" s="22">
+        <f>E36*F36</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="22">
+        <f>1.18*G36</f>
+        <v>0</v>
+      </c>
+      <c r="I36" s="22"/>
+      <c r="J36" s="30"/>
+    </row>
+    <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="17"/>
+      <c r="B37" s="60" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="16"/>
       <c r="D37" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="17"/>
-      <c r="F37" s="23"/>
-      <c r="G37" s="23">
-        <f>E37*F37</f>
-        <v>0</v>
-      </c>
-      <c r="H37" s="23">
-        <f>1.18*G37</f>
-        <v>0</v>
-      </c>
-      <c r="I37" s="23"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="34"/>
-    </row>
-    <row r="38" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="18"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
+      <c r="E37" s="16">
+        <v>0</v>
+      </c>
+      <c r="F37" s="16">
+        <v>0</v>
+      </c>
+      <c r="G37" s="22">
+        <f t="shared" ref="G37:G40" si="7">E37*F37</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="22">
+        <f t="shared" ref="H37:H40" si="8">1.18*G37</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="18"/>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="16"/>
+      <c r="D38" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" s="16">
+        <v>0</v>
+      </c>
+      <c r="F38" s="16">
+        <v>0</v>
+      </c>
+      <c r="G38" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H38" s="22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="I38" s="18"/>
-      <c r="J38" s="18"/>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="18"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="18"/>
-      <c r="H39" s="18"/>
+    </row>
+    <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="16"/>
+      <c r="D39" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E39" s="16">
+        <v>0</v>
+      </c>
+      <c r="F39" s="16">
+        <v>0</v>
+      </c>
+      <c r="G39" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="I39" s="18"/>
-      <c r="J39" s="18"/>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="18"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
+    </row>
+    <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="60"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="16">
+        <v>0</v>
+      </c>
+      <c r="F40" s="16">
+        <v>0</v>
+      </c>
+      <c r="G40" s="22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H40" s="22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
       <c r="I40" s="18"/>
-      <c r="J40" s="18"/>
-    </row>
-    <row r="41" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="B42" s="48"/>
-      <c r="C42" s="48"/>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="48"/>
-      <c r="J42" s="49"/>
-    </row>
-    <row r="43" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="18"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="18"/>
+    </row>
+    <row r="41" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="42"/>
+      <c r="C41" s="42"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="42"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="42"/>
+      <c r="H41" s="42"/>
+      <c r="I41" s="42"/>
+    </row>
+    <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="16"/>
+      <c r="D42" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E42" s="16">
+        <v>0</v>
+      </c>
+      <c r="F42" s="16">
+        <v>0</v>
+      </c>
+      <c r="G42" s="16">
+        <f>E42*F42</f>
+        <v>0</v>
+      </c>
+      <c r="H42" s="16">
+        <f>G42*1.18</f>
+        <v>0</v>
+      </c>
+      <c r="I42" s="18"/>
+    </row>
+    <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="16"/>
+      <c r="D43" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" s="16">
+        <v>0</v>
+      </c>
+      <c r="F43" s="16">
+        <v>0</v>
+      </c>
+      <c r="G43" s="16">
+        <f t="shared" ref="G43:G47" si="9">E43*F43</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="16">
+        <f t="shared" ref="H43:H47" si="10">G43*1.18</f>
+        <v>0</v>
+      </c>
       <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-    </row>
-    <row r="44" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="18"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
+    </row>
+    <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="16"/>
+      <c r="D44" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" s="16">
+        <v>0</v>
+      </c>
+      <c r="F44" s="16">
+        <v>0</v>
+      </c>
+      <c r="G44" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H44" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="I44" s="18"/>
-      <c r="J44" s="18"/>
-    </row>
-    <row r="45" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="18"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
+    </row>
+    <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="16"/>
+      <c r="D45" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="16">
+        <v>0</v>
+      </c>
+      <c r="F45" s="16">
+        <v>0</v>
+      </c>
+      <c r="G45" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H45" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="I45" s="18"/>
-      <c r="J45" s="18"/>
-    </row>
-    <row r="46" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
+    </row>
+    <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="60" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="16"/>
+      <c r="D46" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="16">
+        <v>0</v>
+      </c>
+      <c r="F46" s="16">
+        <v>0</v>
+      </c>
+      <c r="G46" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H46" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
       <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B47" s="17"/>
+    </row>
+    <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="23"/>
       <c r="C47" s="17"/>
       <c r="D47" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E47" s="17"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="23">
-        <f t="shared" ref="G47:G53" si="4">E47*F47</f>
-        <v>0</v>
-      </c>
-      <c r="H47" s="23">
-        <f t="shared" ref="H47:H53" si="5">1.18*G47</f>
-        <v>0</v>
-      </c>
-      <c r="I47" s="23"/>
-      <c r="J47" s="17"/>
-      <c r="K47" s="34"/>
-    </row>
-    <row r="48" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="45"/>
-      <c r="G48" s="45"/>
-      <c r="H48" s="45"/>
-      <c r="I48" s="45"/>
-      <c r="J48" s="46"/>
-      <c r="K48" s="34"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B49" s="17"/>
+      <c r="E47" s="16">
+        <v>0</v>
+      </c>
+      <c r="F47" s="16">
+        <v>0</v>
+      </c>
+      <c r="G47" s="16">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="H47" s="16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="I47" s="22"/>
+      <c r="J47" s="30"/>
+    </row>
+    <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="B48" s="43"/>
+      <c r="C48" s="43"/>
+      <c r="D48" s="43"/>
+      <c r="E48" s="43"/>
+      <c r="F48" s="43"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="43"/>
+      <c r="I48" s="43"/>
+      <c r="J48" s="30"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="17"/>
+      <c r="B49" s="23"/>
       <c r="C49" s="17"/>
-      <c r="D49" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="D49" s="17"/>
       <c r="E49" s="17"/>
       <c r="F49" s="17"/>
-      <c r="G49" s="23">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H49" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I49" s="23"/>
-      <c r="J49" s="17"/>
-      <c r="K49" s="34"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B50" s="17"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="30"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" s="17"/>
       <c r="C50" s="17"/>
-      <c r="D50" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="D50" s="17"/>
       <c r="E50" s="17"/>
       <c r="F50" s="17"/>
-      <c r="G50" s="23">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H50" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I50" s="23"/>
-      <c r="J50" s="17"/>
-      <c r="K50" s="34"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E51" s="17"/>
-      <c r="F51" s="17"/>
-      <c r="G51" s="23">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H51" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I51" s="23"/>
-      <c r="J51" s="17"/>
-      <c r="K51" s="34"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="30"/>
+    </row>
+    <row r="51" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" s="43"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="43"/>
+      <c r="F51" s="43"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="43"/>
+      <c r="I51" s="43"/>
+      <c r="J51" s="30"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B52" s="17"/>
+      <c r="B52" s="23"/>
       <c r="C52" s="17"/>
-      <c r="D52" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="D52" s="17"/>
       <c r="E52" s="17"/>
       <c r="F52" s="17"/>
-      <c r="G52" s="23">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H52" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I52" s="23"/>
-      <c r="J52" s="17"/>
-      <c r="K52" s="34"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G52" s="22">
+        <f t="shared" ref="G47:G56" si="11">E52*F52</f>
+        <v>0</v>
+      </c>
+      <c r="H52" s="22">
+        <f t="shared" ref="H47:H56" si="12">1.18*G52</f>
+        <v>0</v>
+      </c>
+      <c r="I52" s="22"/>
+      <c r="J52" s="30"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B53" s="17"/>
+      <c r="B53" s="23"/>
       <c r="C53" s="17"/>
-      <c r="D53" s="17" t="s">
-        <v>43</v>
-      </c>
+      <c r="D53" s="17"/>
       <c r="E53" s="17"/>
       <c r="F53" s="17"/>
-      <c r="G53" s="23">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H53" s="23">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="I53" s="23"/>
-      <c r="J53" s="17"/>
-      <c r="K53" s="34"/>
-    </row>
-    <row r="54" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="41" t="s">
+      <c r="G53" s="22">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H53" s="22">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="I53" s="22"/>
+      <c r="J53" s="30"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" s="23"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+      <c r="E54" s="17"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="22">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H54" s="22">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="I54" s="22"/>
+      <c r="J54" s="30"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="23"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
+      <c r="F55" s="17"/>
+      <c r="G55" s="22">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H55" s="22">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="I55" s="22"/>
+      <c r="J55" s="30"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="23"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="22">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="H56" s="22">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="I56" s="22"/>
+      <c r="J56" s="30"/>
+    </row>
+    <row r="57" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B54" s="42"/>
-      <c r="C54" s="42"/>
-      <c r="D54" s="42"/>
-      <c r="E54" s="42"/>
-      <c r="F54" s="42"/>
-      <c r="G54" s="43"/>
-      <c r="H54" s="23">
-        <f>SUM(H12:H28)</f>
-        <v>3580.12</v>
-      </c>
-      <c r="I54" s="23">
+      <c r="B57" s="57"/>
+      <c r="C57" s="57"/>
+      <c r="D57" s="57"/>
+      <c r="E57" s="57"/>
+      <c r="F57" s="57"/>
+      <c r="G57" s="57"/>
+      <c r="H57" s="22">
+        <f>SUM(H10:H26)</f>
+        <v>3358.87</v>
+      </c>
+      <c r="I57" s="22">
         <v>5500</v>
       </c>
-      <c r="J54" s="17"/>
-      <c r="K54" s="25"/>
+      <c r="J57" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A36:J36"/>
-    <mergeCell ref="A5:G5"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A48:J48"/>
-    <mergeCell ref="A42:J42"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A18:J18"/>
-    <mergeCell ref="A23:J23"/>
-    <mergeCell ref="A30:J30"/>
+  <mergeCells count="12">
+    <mergeCell ref="A35:I35"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A57:G57"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A51:I51"/>
+    <mergeCell ref="A41:I41"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A16:I16"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="A29:I29"/>
+    <mergeCell ref="A48:I48"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K32" r:id="rId1"/>
-    <hyperlink ref="K25" r:id="rId2"/>
-    <hyperlink ref="K19" r:id="rId3"/>
-    <hyperlink ref="K13" r:id="rId4"/>
-    <hyperlink ref="K16" r:id="rId5"/>
+    <hyperlink ref="J31" r:id="rId1"/>
+    <hyperlink ref="J23" r:id="rId2"/>
+    <hyperlink ref="J17" r:id="rId3"/>
+    <hyperlink ref="J11" r:id="rId4"/>
+    <hyperlink ref="J14" r:id="rId5"/>
+    <hyperlink ref="J15" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -2240,15 +2509,15 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="55"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="46"/>
       <c r="H5" s="8">
         <f>SUM(H2:H4)</f>
         <v>6608</v>
@@ -2630,15 +2899,15 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="58"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="49"/>
       <c r="H19" s="8">
         <f>SUM(H7:H18)</f>
         <v>3091.6</v>
@@ -2759,15 +3028,15 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="58"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="49"/>
       <c r="H25" s="9">
         <f>SUM(H21:H24)</f>
         <v>5900</v>
@@ -2932,15 +3201,15 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="55"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="46"/>
       <c r="H5" s="8">
         <f>SUM(H2:H4)</f>
         <v>6608</v>
@@ -3322,15 +3591,15 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="58"/>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="49"/>
       <c r="H19" s="8">
         <f>SUM(H7:H18)</f>
         <v>5097.5999999999995</v>
@@ -3451,15 +3720,15 @@
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="58"/>
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="49"/>
       <c r="H25" s="9">
         <f>SUM(H21:H24)</f>
         <v>5900</v>
@@ -3491,32 +3760,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
-        <v>75</v>
+      <c r="A2" s="35" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
-        <v>74</v>
+      <c r="A3" s="35" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
-        <v>79</v>
+      <c r="A5" s="35" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39" t="s">
-        <v>80</v>
+      <c r="A6" s="35" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>